<commit_message>
Added Sql test cases
</commit_message>
<xml_diff>
--- a/Test Cases Final/TC- 4 Dashboard.xlsx
+++ b/Test Cases Final/TC- 4 Dashboard.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cror\Desktop\Test Cases\Test Cases Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9B8620-132C-4FD6-A908-2B36168BCED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBD030E-E476-45FA-B6E4-953B5571280B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TEST CASE TEMPLATE" sheetId="5" r:id="rId1"/>
+    <sheet name="TC_Dashboard" sheetId="5" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -900,7 +901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B15" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B14" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
@@ -1850,4 +1851,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8680C67-F3F1-4A48-B89A-BB176A562065}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>